<commit_message>
Anes first attempt to make a form
</commit_message>
<xml_diff>
--- a/app/config/tables/OPVCOVIDHC/Forms/OPVCOVIDHC/OPVCOVIDHC.xlsx
+++ b/app/config/tables/OPVCOVIDHC/Forms/OPVCOVIDHC/OPVCOVIDHC.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DCF458-26C3-4892-B624-494D0ADDA068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DBB059-402B-4CCA-871B-7BEF1DAEB808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="140">
   <si>
     <t>setting_name</t>
   </si>
@@ -167,12 +167,6 @@
     <t>display.constraint_message.text</t>
   </si>
   <si>
-    <t>This is the first screen</t>
-  </si>
-  <si>
-    <t>Esta é a primeira tela</t>
-  </si>
-  <si>
     <t>OPVCOVID: Health center follow-up</t>
   </si>
   <si>
@@ -182,10 +176,283 @@
     <t>OPVCOVIDHC</t>
   </si>
   <si>
-    <t>Next screen</t>
-  </si>
-  <si>
-    <t>Próxima tela</t>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>select_one</t>
+  </si>
+  <si>
+    <t>C_IDENT</t>
+  </si>
+  <si>
+    <t>C_NAME</t>
+  </si>
+  <si>
+    <t>C_DATE</t>
+  </si>
+  <si>
+    <t>C_NUMEST</t>
+  </si>
+  <si>
+    <t>C_IDENTDATE</t>
+  </si>
+  <si>
+    <t>C_CERTEZA</t>
+  </si>
+  <si>
+    <t>C_SYMPTOMS</t>
+  </si>
+  <si>
+    <t>C_TEST</t>
+  </si>
+  <si>
+    <t>C_TEST1Q</t>
+  </si>
+  <si>
+    <t>C_TEST1RES</t>
+  </si>
+  <si>
+    <t>C_TEST2RES</t>
+  </si>
+  <si>
+    <t>C_TEST2Q</t>
+  </si>
+  <si>
+    <t>C_DIAGN1</t>
+  </si>
+  <si>
+    <t>C_DIAGN2</t>
+  </si>
+  <si>
+    <t>C_DIAGN3</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text </t>
+  </si>
+  <si>
+    <t>YesNoUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Don't know</t>
+  </si>
+  <si>
+    <t>Não sabe</t>
+  </si>
+  <si>
+    <t>Missing information</t>
+  </si>
+  <si>
+    <t>Falta informação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data: </t>
+  </si>
+  <si>
+    <t>Reciept</t>
+  </si>
+  <si>
+    <t>Recibo</t>
+  </si>
+  <si>
+    <t>Nome na recibo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numest; PC: </t>
+  </si>
+  <si>
+    <t>Identified in the consultation Book?</t>
+  </si>
+  <si>
+    <t>A pessoa foi identificado na livro de consulta?</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>data('C_IDENT') == '1'</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>Data na Livro:</t>
+  </si>
+  <si>
+    <t>Identificacao certo?</t>
+  </si>
+  <si>
+    <t>Quais sintomas?</t>
+  </si>
+  <si>
+    <t>Teste realisado?</t>
+  </si>
+  <si>
+    <t>Qual teste</t>
+  </si>
+  <si>
+    <t>Resultado de teste?</t>
+  </si>
+  <si>
+    <t>data('C_TEST') == '1'</t>
+  </si>
+  <si>
+    <t>Outro teste?</t>
+  </si>
+  <si>
+    <t>C_TEST2</t>
+  </si>
+  <si>
+    <t>Symptoms</t>
+  </si>
+  <si>
+    <t>TestResult</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Positivo</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Negativo</t>
+  </si>
+  <si>
+    <t>Don't know yet</t>
+  </si>
+  <si>
+    <t>Ainda não sabe</t>
+  </si>
+  <si>
+    <t>Tosse</t>
+  </si>
+  <si>
+    <t>Febre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diarreia </t>
+  </si>
+  <si>
+    <t>Vomito</t>
+  </si>
+  <si>
+    <t>Falta de ar</t>
+  </si>
+  <si>
+    <t>Rinorreia</t>
+  </si>
+  <si>
+    <t>Dor de garganta</t>
+  </si>
+  <si>
+    <t>Convulsao</t>
+  </si>
+  <si>
+    <t>C_SYMPTOUTR</t>
+  </si>
+  <si>
+    <t>C_SYMPTQUAIS</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>TestType</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>TDR</t>
+  </si>
+  <si>
+    <t>Leuko</t>
+  </si>
+  <si>
+    <t>Hb</t>
+  </si>
+  <si>
+    <t>Not categoric</t>
+  </si>
+  <si>
+    <t>Nao Categorico</t>
+  </si>
+  <si>
+    <t>C_TEST1RESC</t>
+  </si>
+  <si>
+    <t>C_TEST2RESC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if </t>
+  </si>
+  <si>
+    <t>data('C_TEST1RESC') == '4'</t>
+  </si>
+  <si>
+    <t>Outras sintomas?</t>
+  </si>
+  <si>
+    <t>data('C_SYMPTOUTR')=='1'</t>
+  </si>
+  <si>
+    <t>Which symptoms</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>C_TEST1QOUT</t>
+  </si>
+  <si>
+    <t>C_TEST2QOUT</t>
+  </si>
+  <si>
+    <t>data('C_TEST1Q') == '8'</t>
+  </si>
+  <si>
+    <t>Qual</t>
+  </si>
+  <si>
+    <t>Qual?</t>
+  </si>
+  <si>
+    <t>c_TEST1QOUT</t>
+  </si>
+  <si>
+    <t>data('C_TEST2') == '1'</t>
+  </si>
+  <si>
+    <t>data('C_TEST2Q') == '8'</t>
+  </si>
+  <si>
+    <t>c_TEST2QOUT</t>
+  </si>
+  <si>
+    <t>data('C_TEST2RESC') == '4'</t>
   </si>
 </sst>
 </file>
@@ -276,7 +543,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -289,6 +556,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -576,20 +845,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -609,43 +878,43 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>14082020</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>270820</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -656,7 +925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -667,7 +936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
@@ -686,138 +955,633 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787AB6FC-E5B2-448F-8A60-6571052C1548}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.81640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.1796875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" style="11" customWidth="1"/>
+    <col min="11" max="11" width="37.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="G3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="E18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="11" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D25" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D28" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D33" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D36" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D37" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D39" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D40" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D42" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D45" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B50" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D51" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D52" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D54" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D55" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B56" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D57" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D58" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B59" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D60" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D61" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B62" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D63" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="11" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -831,261 +1595,582 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"9"</f>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"8"</f>
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="str">
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="str">
+        <f>"7"</f>
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="str">
+        <f>"8"</f>
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="str">
+        <f>"9"</f>
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="str">
+        <f>"10"</f>
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="str">
+        <f>"11"</f>
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="7"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="7"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="7"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="7"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="7"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="7"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="7"/>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" s="7"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="7"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="7"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="7"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="7"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" s="7"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" s="7"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72" s="7"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" s="7"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" s="7"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" s="7"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" s="7"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" s="7"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" s="7"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="7"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="7"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="7"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1103,13 +2188,13 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1132,15 +2217,15 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -1154,7 +2239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1176,21 +2261,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1199,6 +2284,248 @@
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to diagnoses and treatment
</commit_message>
<xml_diff>
--- a/app/config/tables/OPVCOVIDHC/Forms/OPVCOVIDHC/OPVCOVIDHC.xlsx
+++ b/app/config/tables/OPVCOVIDHC/Forms/OPVCOVIDHC/OPVCOVIDHC.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F94CE00-7A61-47DE-9584-A804F4E074D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B2215A-F7DC-4A49-A222-C6747BA3A088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="278">
   <si>
     <t>setting_name</t>
   </si>
@@ -846,6 +846,27 @@
   </si>
   <si>
     <t>Gastritis / Ulcera gastroduodenal</t>
+  </si>
+  <si>
+    <t>Febre Tifoide</t>
+  </si>
+  <si>
+    <t>Ciprofloxacin</t>
+  </si>
+  <si>
+    <t>Ciprofloxacina</t>
+  </si>
+  <si>
+    <t>Iron FA</t>
+  </si>
+  <si>
+    <t>Sulfato Feroso</t>
+  </si>
+  <si>
+    <t>Complexo B</t>
+  </si>
+  <si>
+    <t>Infeccao urinaria</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787AB6FC-E5B2-448F-8A60-6571052C1548}">
   <dimension ref="A1:M163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+    <sheetView zoomScale="117" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
@@ -2918,11 +2939,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView zoomScale="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3681,14 +3702,14 @@
         <v>129</v>
       </c>
       <c r="B55" t="str">
-        <f>"77"</f>
-        <v>77</v>
+        <f>"16"</f>
+        <v>16</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>116</v>
+        <v>271</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>116</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -3696,44 +3717,44 @@
         <v>129</v>
       </c>
       <c r="B56" t="str">
+        <f>"17"</f>
+        <v>17</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" t="str">
+        <f>"77"</f>
+        <v>77</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D58" s="7" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>130</v>
-      </c>
-      <c r="B57" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>130</v>
-      </c>
-      <c r="B58" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -3741,14 +3762,14 @@
         <v>130</v>
       </c>
       <c r="B59" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>227</v>
+        <v>131</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>227</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -3756,14 +3777,14 @@
         <v>130</v>
       </c>
       <c r="B60" t="str">
-        <f>"4"</f>
-        <v>4</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -3771,14 +3792,14 @@
         <v>130</v>
       </c>
       <c r="B61" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -3786,14 +3807,14 @@
         <v>130</v>
       </c>
       <c r="B62" t="str">
-        <f>"6"</f>
-        <v>6</v>
+        <f>"4"</f>
+        <v>4</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -3801,14 +3822,14 @@
         <v>130</v>
       </c>
       <c r="B63" t="str">
-        <f>"7"</f>
-        <v>7</v>
+        <f>"5"</f>
+        <v>5</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -3816,14 +3837,14 @@
         <v>130</v>
       </c>
       <c r="B64" t="str">
-        <f>"8"</f>
-        <v>8</v>
+        <f>"6"</f>
+        <v>6</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -3831,14 +3852,14 @@
         <v>130</v>
       </c>
       <c r="B65" t="str">
-        <f>"9"</f>
-        <v>9</v>
+        <f>"7"</f>
+        <v>7</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -3846,14 +3867,14 @@
         <v>130</v>
       </c>
       <c r="B66" t="str">
-        <f>"10"</f>
-        <v>10</v>
+        <f>"8"</f>
+        <v>8</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -3861,14 +3882,14 @@
         <v>130</v>
       </c>
       <c r="B67" t="str">
-        <f>"11"</f>
-        <v>11</v>
+        <f>"9"</f>
+        <v>9</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -3876,14 +3897,14 @@
         <v>130</v>
       </c>
       <c r="B68" t="str">
-        <f>"12"</f>
-        <v>12</v>
+        <f>"10"</f>
+        <v>10</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -3891,14 +3912,14 @@
         <v>130</v>
       </c>
       <c r="B69" t="str">
-        <f>"13"</f>
-        <v>13</v>
+        <f>"11"</f>
+        <v>11</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -3906,14 +3927,14 @@
         <v>130</v>
       </c>
       <c r="B70" t="str">
-        <f>"14"</f>
-        <v>14</v>
+        <f>"12"</f>
+        <v>12</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -3921,14 +3942,14 @@
         <v>130</v>
       </c>
       <c r="B71" t="str">
-        <f>"15"</f>
-        <v>15</v>
+        <f>"13"</f>
+        <v>13</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -3936,14 +3957,14 @@
         <v>130</v>
       </c>
       <c r="B72" t="str">
-        <f>"16"</f>
-        <v>16</v>
+        <f>"14"</f>
+        <v>14</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -3951,14 +3972,14 @@
         <v>130</v>
       </c>
       <c r="B73" t="str">
-        <f>"17"</f>
-        <v>17</v>
+        <f>"15"</f>
+        <v>15</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -3966,14 +3987,14 @@
         <v>130</v>
       </c>
       <c r="B74" t="str">
-        <f>"18"</f>
-        <v>18</v>
+        <f>"16"</f>
+        <v>16</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -3981,14 +4002,14 @@
         <v>130</v>
       </c>
       <c r="B75" t="str">
-        <f>"19"</f>
-        <v>19</v>
+        <f>"17"</f>
+        <v>17</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
@@ -3996,14 +4017,14 @@
         <v>130</v>
       </c>
       <c r="B76" t="str">
-        <f>"20"</f>
-        <v>20</v>
+        <f>"18"</f>
+        <v>18</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -4011,14 +4032,14 @@
         <v>130</v>
       </c>
       <c r="B77" t="str">
-        <f>"21"</f>
-        <v>21</v>
+        <f>"19"</f>
+        <v>19</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -4026,14 +4047,14 @@
         <v>130</v>
       </c>
       <c r="B78" t="str">
-        <f>"22"</f>
-        <v>22</v>
+        <f>"20"</f>
+        <v>20</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -4041,14 +4062,14 @@
         <v>130</v>
       </c>
       <c r="B79" t="str">
-        <f>"23"</f>
-        <v>23</v>
+        <f>"21"</f>
+        <v>21</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -4056,14 +4077,14 @@
         <v>130</v>
       </c>
       <c r="B80" t="str">
-        <f>"24"</f>
-        <v>24</v>
+        <f>"22"</f>
+        <v>22</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -4071,14 +4092,14 @@
         <v>130</v>
       </c>
       <c r="B81" t="str">
-        <f>"25"</f>
-        <v>25</v>
+        <f>"23"</f>
+        <v>23</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
@@ -4086,14 +4107,14 @@
         <v>130</v>
       </c>
       <c r="B82" t="str">
-        <f>"26"</f>
-        <v>26</v>
+        <f>"24"</f>
+        <v>24</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
@@ -4101,14 +4122,14 @@
         <v>130</v>
       </c>
       <c r="B83" t="str">
-        <f>"27"</f>
-        <v>27</v>
+        <f>"25"</f>
+        <v>25</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
@@ -4116,14 +4137,14 @@
         <v>130</v>
       </c>
       <c r="B84" t="str">
-        <f>"28"</f>
-        <v>28</v>
+        <f>"26"</f>
+        <v>26</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
@@ -4131,50 +4152,105 @@
         <v>130</v>
       </c>
       <c r="B85" t="str">
-        <f>"77"</f>
-        <v>77</v>
+        <f>"27"</f>
+        <v>27</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>116</v>
+        <v>268</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>116</v>
+        <v>268</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>130</v>
       </c>
-      <c r="B86" s="7" t="str">
+      <c r="B86" t="str">
+        <f>"28"</f>
+        <v>28</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>130</v>
+      </c>
+      <c r="B87" t="str">
+        <f>"29"</f>
+        <v>29</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B88" t="str">
+        <f>"30"</f>
+        <v>30</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>130</v>
+      </c>
+      <c r="B89" t="str">
+        <f>"31"</f>
+        <v>31</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>130</v>
+      </c>
+      <c r="B90" t="str">
+        <f>"77"</f>
+        <v>77</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>130</v>
+      </c>
+      <c r="B91" s="7" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C91" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D91" s="7" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B92" s="7"/>
@@ -4182,59 +4258,64 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B96" s="7"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C96" s="7"/>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" s="7"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C97" s="7"/>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98" s="7"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" s="7"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B100" s="7"/>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101" s="7"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102" s="7"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103" s="7"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" s="7"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B105" s="7"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106" s="7"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" s="7"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108" s="7"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109" s="7"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110" s="7"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111" s="7"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112" s="7"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.35">
@@ -4254,6 +4335,21 @@
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B118" s="7"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B119" s="7"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B120" s="7"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B121" s="7"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B122" s="7"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B123" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Addition of option to add health center
</commit_message>
<xml_diff>
--- a/app/config/tables/OPVCOVIDHC/Forms/OPVCOVIDHC/OPVCOVIDHC.xlsx
+++ b/app/config/tables/OPVCOVIDHC/Forms/OPVCOVIDHC/OPVCOVIDHC.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B2215A-F7DC-4A49-A222-C6747BA3A088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F359B3A2-3BF9-4B26-BE06-FE69A0694434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="675" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="284">
   <si>
     <t>setting_name</t>
   </si>
@@ -867,6 +867,24 @@
   </si>
   <si>
     <t>Infeccao urinaria</t>
+  </si>
+  <si>
+    <t>C_CS</t>
+  </si>
+  <si>
+    <t>Health Center</t>
+  </si>
+  <si>
+    <t>Centro de Saude</t>
+  </si>
+  <si>
+    <t>Centro</t>
+  </si>
+  <si>
+    <t>CS Bandim</t>
+  </si>
+  <si>
+    <t>CS Cuntum</t>
   </si>
 </sst>
 </file>
@@ -1391,12 +1409,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787AB6FC-E5B2-448F-8A60-6571052C1548}">
-  <dimension ref="A1:M163"/>
+  <dimension ref="A1:M164"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1465,377 +1483,389 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H4" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D5" s="11" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D7" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D8" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>76</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B11" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="11" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B12" s="11" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D13" s="11" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D15" s="11" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B16" s="11" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="11" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D19" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D22" s="11" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D23" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E23" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H23" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D24" s="11" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D25" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B26" s="11" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D27" s="11" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D28" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H28" s="11" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="11" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D31" s="11" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D32" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G32" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H32" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="12" t="s">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C33" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B33" s="12"/>
-      <c r="D33" s="11" t="s">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="12"/>
+      <c r="D34" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E34" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H34" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B34" s="12" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B35" s="12"/>
-      <c r="D35" s="11" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="12"/>
+      <c r="D36" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F36" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G36" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H36" s="11" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B36" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B38" s="12"/>
-      <c r="D38" s="11" t="s">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B39" s="12"/>
+      <c r="D39" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F39" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B39" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="12"/>
-      <c r="D41" s="11" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="12"/>
+      <c r="D42" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F42" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G42" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H41" s="11" t="s">
+      <c r="H42" s="11" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B42" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.35">
@@ -1844,153 +1874,153 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B44" s="11" t="s">
-        <v>40</v>
+      <c r="B44" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13" t="s">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E48" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F48" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="G48" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B48" s="11" t="s">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B49" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C49" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B49" s="12"/>
-      <c r="D49" s="11" t="s">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B50" s="12"/>
+      <c r="D50" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G50" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B50" s="12" t="s">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B51" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C51" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B51" s="12"/>
-      <c r="D51" s="11" t="s">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B52" s="12"/>
+      <c r="D52" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F52" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G52" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H52" s="11" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B52" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C54" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B54" s="12"/>
-      <c r="D54" s="11" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="12"/>
+      <c r="D55" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G55" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H55" s="11" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B55" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B56" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C57" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B57" s="12"/>
-      <c r="D57" s="11" t="s">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B58" s="12"/>
+      <c r="D58" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F58" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G58" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H57" s="11" t="s">
+      <c r="H58" s="11" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B58" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.35">
@@ -1999,158 +2029,158 @@
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B61" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B61" s="12" t="s">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B62" s="12" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B62" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B63" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13" t="s">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E64" s="13" t="s">
+      <c r="E65" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="13" t="s">
+      <c r="F65" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="G64" s="13" t="s">
+      <c r="G65" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="H64" s="11" t="s">
+      <c r="H65" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="11" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C66" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="12"/>
-      <c r="D66" s="11" t="s">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="12"/>
+      <c r="D67" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E67" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F67" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G67" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H66" s="11" t="s">
+      <c r="H67" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="12" t="s">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C68" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B68" s="12"/>
-      <c r="D68" s="11" t="s">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B69" s="12"/>
+      <c r="D69" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F68" s="11" t="s">
+      <c r="F69" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="G68" s="11" t="s">
+      <c r="G69" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H68" s="11" t="s">
+      <c r="H69" s="11" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B69" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B70" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B71" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C71" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B71" s="12"/>
-      <c r="D71" s="11" t="s">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B72" s="12"/>
+      <c r="D72" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="E72" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F71" s="11" t="s">
+      <c r="F72" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H71" s="11" t="s">
+      <c r="H72" s="11" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B72" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B73" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B74" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C74" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B74" s="12"/>
-      <c r="D74" s="11" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B75" s="12"/>
+      <c r="D75" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="F75" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="G75" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H74" s="11" t="s">
+      <c r="H75" s="11" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B75" s="12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.35">
@@ -2159,775 +2189,780 @@
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B78" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B78" s="12" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B79" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B79" s="11" t="s">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B80" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D80" s="11" t="s">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D81" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E81" t="s">
         <v>129</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>150</v>
       </c>
-      <c r="G80" s="11" t="s">
+      <c r="G81" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="H80" s="11" t="s">
+      <c r="H81" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B81" s="11" t="s">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B82" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C82" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D82" s="11" t="s">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D83" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E82"/>
-      <c r="F82" t="s">
+      <c r="E83"/>
+      <c r="F83" t="s">
         <v>157</v>
       </c>
-      <c r="G82" s="11" t="s">
+      <c r="G83" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H82" s="11" t="s">
+      <c r="H83" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B83" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E83"/>
-      <c r="F83"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B84" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E84"/>
       <c r="F84"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B85" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E85"/>
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B86" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C86" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B87" s="11" t="s">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B88" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D88" s="11" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D89" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E89" t="s">
         <v>129</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F89" t="s">
         <v>151</v>
       </c>
-      <c r="G88" s="11" t="s">
+      <c r="G89" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="H88" s="11" t="s">
+      <c r="H89" s="11" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B89" s="11" t="s">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B90" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C90" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D90" s="11" t="s">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D91" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E90"/>
-      <c r="F90" t="s">
+      <c r="E91"/>
+      <c r="F91" t="s">
         <v>160</v>
       </c>
-      <c r="G90" s="11" t="s">
+      <c r="G91" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H90" s="11" t="s">
+      <c r="H91" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B91" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E91"/>
-      <c r="F91"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B92" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E92"/>
       <c r="F92"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B93" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E93"/>
+      <c r="F93"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B94" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>163</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B95" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B96" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D96" s="11" t="s">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D97" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E97" t="s">
         <v>129</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F97" t="s">
         <v>161</v>
       </c>
-      <c r="G96" s="11" t="s">
+      <c r="G97" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="H96" s="11" t="s">
+      <c r="H97" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B97" s="11" t="s">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B98" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C98" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D98" s="11" t="s">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D99" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E98"/>
-      <c r="F98" t="s">
+      <c r="E99"/>
+      <c r="F99" t="s">
         <v>162</v>
       </c>
-      <c r="G98" s="11" t="s">
+      <c r="G99" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H98" s="11" t="s">
+      <c r="H99" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B99" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E99"/>
-      <c r="F99"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B100" s="11" t="s">
-        <v>40</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E100"/>
+      <c r="F100"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B101" s="11" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B102" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B103" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D103" s="11" t="s">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D104" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E104" t="s">
         <v>130</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F104" t="s">
         <v>166</v>
       </c>
-      <c r="G103" s="11" t="s">
+      <c r="G104" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="H103" s="11" t="s">
+      <c r="H104" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B104" s="11" t="s">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B105" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C105" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D105" s="11" t="s">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D106" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E105"/>
-      <c r="F105" t="s">
+      <c r="E106"/>
+      <c r="F106" t="s">
         <v>173</v>
       </c>
-      <c r="G105" s="11" t="s">
+      <c r="G106" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H105" s="11" t="s">
+      <c r="H106" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B106" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E106"/>
-      <c r="F106"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B107" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E107"/>
       <c r="F107"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B108" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>176</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E108"/>
+      <c r="F108"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B109" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B110" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D110" s="11" t="s">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D111" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E111" t="s">
         <v>130</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F111" t="s">
         <v>167</v>
       </c>
-      <c r="G110" s="11" t="s">
+      <c r="G111" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="H110" s="11" t="s">
+      <c r="H111" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B111" s="11" t="s">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B112" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C112" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D112" s="11" t="s">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D113" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E112"/>
-      <c r="F112" t="s">
+      <c r="E113"/>
+      <c r="F113" t="s">
         <v>178</v>
       </c>
-      <c r="G112" s="11" t="s">
+      <c r="G113" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H112" s="11" t="s">
+      <c r="H113" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B113" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E113"/>
-      <c r="F113"/>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B114" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E114"/>
       <c r="F114"/>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B115" s="11" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E115"/>
       <c r="F115"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B116" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>196</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E116"/>
+      <c r="F116"/>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B117" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C117" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B118" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D118" s="11" t="s">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D119" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E119" t="s">
         <v>130</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F119" t="s">
         <v>168</v>
       </c>
-      <c r="G118" s="11" t="s">
+      <c r="G119" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="H118" s="11" t="s">
+      <c r="H119" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B119" s="11" t="s">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B120" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C119" s="11" t="s">
+      <c r="C120" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D120" s="11" t="s">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D121" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E120"/>
-      <c r="F120" t="s">
+      <c r="E121"/>
+      <c r="F121" t="s">
         <v>189</v>
       </c>
-      <c r="G120" s="11" t="s">
+      <c r="G121" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H120" s="11" t="s">
+      <c r="H121" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B121" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E121"/>
-      <c r="F121"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B122" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E122"/>
       <c r="F122"/>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B123" s="11" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E123"/>
       <c r="F123"/>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B124" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C124" s="11" t="s">
-        <v>197</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E124"/>
+      <c r="F124"/>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B125" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B126" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D126" s="11" t="s">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D127" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E127" t="s">
         <v>130</v>
       </c>
-      <c r="F126" t="s">
+      <c r="F127" t="s">
         <v>169</v>
       </c>
-      <c r="G126" s="11" t="s">
+      <c r="G127" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="H126" s="11" t="s">
+      <c r="H127" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B127" s="11" t="s">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B128" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C128" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D128" s="11" t="s">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D129" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E128"/>
-      <c r="F128" t="s">
+      <c r="E129"/>
+      <c r="F129" t="s">
         <v>188</v>
       </c>
-      <c r="G128" s="11" t="s">
+      <c r="G129" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H128" s="11" t="s">
+      <c r="H129" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B129" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E129"/>
-      <c r="F129"/>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B130" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E130"/>
       <c r="F130"/>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B131" s="11" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E131"/>
       <c r="F131"/>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B132" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C132" s="11" t="s">
-        <v>198</v>
+        <v>80</v>
       </c>
       <c r="E132"/>
       <c r="F132"/>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B133" s="11" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="C133" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="E133"/>
       <c r="F133"/>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D135" s="11" t="s">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B134" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E134"/>
+      <c r="F134"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D136" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E136" t="s">
         <v>130</v>
       </c>
-      <c r="F135" t="s">
+      <c r="F136" t="s">
         <v>170</v>
       </c>
-      <c r="G135" s="11" t="s">
+      <c r="G136" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="H135" s="11" t="s">
+      <c r="H136" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B136" s="11" t="s">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B137" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C136" s="11" t="s">
+      <c r="C137" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D137" s="11" t="s">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D138" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E137"/>
-      <c r="F137" t="s">
+      <c r="E138"/>
+      <c r="F138" t="s">
         <v>187</v>
       </c>
-      <c r="G137" s="11" t="s">
+      <c r="G138" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H137" s="11" t="s">
+      <c r="H138" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B138" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E138"/>
-      <c r="F138"/>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B139" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E139"/>
       <c r="F139"/>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B140" s="11" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E140"/>
       <c r="F140"/>
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B141" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C141" s="11" t="s">
-        <v>199</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E141"/>
+      <c r="F141"/>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B142" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B143" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D143" s="11" t="s">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D144" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E144" t="s">
         <v>130</v>
       </c>
-      <c r="F143" t="s">
+      <c r="F144" t="s">
         <v>171</v>
       </c>
-      <c r="G143" s="11" t="s">
+      <c r="G144" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="H143" s="11" t="s">
+      <c r="H144" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B144" s="11" t="s">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B145" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C145" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D145" s="11" t="s">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D146" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E145"/>
-      <c r="F145" t="s">
+      <c r="E146"/>
+      <c r="F146" t="s">
         <v>186</v>
       </c>
-      <c r="G145" s="11" t="s">
+      <c r="G146" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H145" s="11" t="s">
+      <c r="H146" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B146" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E146"/>
-      <c r="F146"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B147" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E147"/>
       <c r="F147"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B148" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E148"/>
+      <c r="F148"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B149" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C149" s="11" t="s">
-        <v>200</v>
+        <v>80</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B150" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B151" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D151" s="11" t="s">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D152" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E152" t="s">
         <v>130</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F152" t="s">
         <v>172</v>
       </c>
-      <c r="G151" s="11" t="s">
+      <c r="G152" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="H151" s="11" t="s">
+      <c r="H152" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B152" s="11" t="s">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B153" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C152" s="11" t="s">
+      <c r="C153" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D153" s="11" t="s">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D154" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E153"/>
-      <c r="F153" t="s">
+      <c r="E154"/>
+      <c r="F154" t="s">
         <v>185</v>
       </c>
-      <c r="G153" s="11" t="s">
+      <c r="G154" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H153" s="11" t="s">
+      <c r="H154" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B154" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E154"/>
-      <c r="F154"/>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B155" s="11" t="s">
-        <v>40</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E155"/>
+      <c r="F155"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B156" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B157" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D157" s="11" t="s">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D158" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E158" t="s">
         <v>64</v>
       </c>
-      <c r="F157" s="11" t="s">
+      <c r="F158" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="G157" s="11" t="s">
+      <c r="G158" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="H157" s="11" t="s">
+      <c r="H158" s="11" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B158" s="11" t="s">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B159" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C158" s="11" t="s">
+      <c r="C159" s="11" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A159" s="14"/>
-      <c r="D159" s="11" t="s">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A160" s="14"/>
+      <c r="D160" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E159"/>
-      <c r="F159" t="s">
+      <c r="E160"/>
+      <c r="F160" t="s">
         <v>255</v>
       </c>
-      <c r="G159" s="11" t="s">
+      <c r="G160" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H159" s="11" t="s">
+      <c r="H160" s="11" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B160" s="11" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B161" s="11" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B162" s="11" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B163" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B164" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2941,9 +2976,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+    <sheetView zoomScale="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4257,12 +4292,34 @@
       <c r="C92" s="7"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
+      <c r="A93" t="s">
+        <v>281</v>
+      </c>
+      <c r="B93" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
+      <c r="A94" t="s">
+        <v>281</v>
+      </c>
+      <c r="B94" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B95" s="7"/>
@@ -4440,11 +4497,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56:C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4994,6 +5051,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>278</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>